<commit_message>
US-12415 [FIX] IR product list import/export: Added 4 columns in the import/export, and a warning on the export popup
</commit_message>
<xml_diff>
--- a/bin/addons/procurement_request/report/ir_product_list_export.xlsx
+++ b/bin/addons/procurement_request/report/ir_product_list_export.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>INTERNAL REQUEST</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>Details</t>
+  </si>
+  <si>
+    <t>Cost Price</t>
+  </si>
+  <si>
+    <t>UoM</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>PCE</t>
+  </si>
+  <si>
+    <t>EUR</t>
   </si>
 </sst>
 </file>
@@ -123,11 +141,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -146,6 +161,21 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -428,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,110 +469,168 @@
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="57.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="4" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="57.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="7"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="3"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>5</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="3">
         <v>25569</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="8"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 D2:G2">
       <formula1>"Normal,Emergency,Priority"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
US-13308 [IMP] FO/IR: Fixed RDD name in doc and reports
</commit_message>
<xml_diff>
--- a/bin/addons/procurement_request/report/ir_product_list_export.xlsx
+++ b/bin/addons/procurement_request/report/ir_product_list_export.xlsx
@@ -27,9 +27,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Requested Date</t>
-  </si>
-  <si>
     <t>Requestor</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>EUR</t>
+  </si>
+  <si>
+    <t>Requested Delivery Date</t>
   </si>
 </sst>
 </file>
@@ -163,20 +163,20 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,7 +461,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,16 +475,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -492,131 +492,131 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C10" s="8">
         <v>5</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="11">
         <v>1.5</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="3">
         <v>25569</v>

</xml_diff>